<commit_message>
Versión para entrega intermedia
</commit_message>
<xml_diff>
--- a/Contenido_Encovi_Departamentales.xlsx
+++ b/Contenido_Encovi_Departamentales.xlsx
@@ -436,7 +436,7 @@
     <t xml:space="preserve">Población ocupada por actividad económica</t>
   </si>
   <si>
-    <t xml:space="preserve">Distribución de la población ocupada según rama de actividad económica por área de residencia</t>
+    <t xml:space="preserve">Distribución de la población ocupada según rama de actividad económica</t>
   </si>
   <si>
     <t xml:space="preserve">Población ocupada por tipo de ocupación</t>
@@ -750,23 +750,23 @@
   </sheetPr>
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="E10" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="topRight" activeCell="J38" activeCellId="0" sqref="J38"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B38" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="topRight" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.4591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="76.9438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="65.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="76.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="64.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>